<commit_message>
Wed Mar 24 18:47:09 PDT 2021
</commit_message>
<xml_diff>
--- a/Resources/StreamLine Web Automator Resources/Actions and Keywords Dictionary.xlsx
+++ b/Resources/StreamLine Web Automator Resources/Actions and Keywords Dictionary.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22527"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23127"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Admin\Desktop\StreamLineQA-Automation\Resources\StreamLine Web Automator Resources\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Admin\Desktop\StreamLineQA-Automation-Test\Resources\StreamLine Web Automator Resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3F703796-620A-4AA3-8C90-FDF8DC3E6A0C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4B5C8A77-6C9B-45F0-80F2-749272415E18}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -308,7 +308,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="380" uniqueCount="252">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="369" uniqueCount="246">
   <si>
     <t>Compare</t>
   </si>
@@ -334,9 +334,6 @@
     <t>delay</t>
   </si>
   <si>
-    <t>compare link custom</t>
-  </si>
-  <si>
     <t>compare css value (css)</t>
   </si>
   <si>
@@ -352,9 +349,6 @@
     <t>home</t>
   </si>
   <si>
-    <t>compare text custom</t>
-  </si>
-  <si>
     <t>compare size</t>
   </si>
   <si>
@@ -400,9 +394,6 @@
     <t>wait until clickable</t>
   </si>
   <si>
-    <t>compare text unformatted</t>
-  </si>
-  <si>
     <t>type value</t>
   </si>
   <si>
@@ -505,9 +496,6 @@
     <t>key up</t>
   </si>
   <si>
-    <t>compare inner html custom</t>
-  </si>
-  <si>
     <t>size x lteq</t>
   </si>
   <si>
@@ -589,15 +577,9 @@
     <t>expected url</t>
   </si>
   <si>
-    <t>Expected value of N/A when element has no link</t>
-  </si>
-  <si>
     <t>expected text</t>
   </si>
   <si>
-    <t>VISIBLE TEXT ONLY. Removes &amp;nbsp;, leading and trailing spaces, and 1 trailing new line character</t>
-  </si>
-  <si>
     <t>yes or no</t>
   </si>
   <si>
@@ -610,9 +592,6 @@
     <t>Scrolls to a given element.</t>
   </si>
   <si>
-    <t>VISIBLE TEXT ONLY</t>
-  </si>
-  <si>
     <t>(x, y)</t>
   </si>
   <si>
@@ -646,18 +625,6 @@
     <t>expected value</t>
   </si>
   <si>
-    <t>domain/ functionality. Pass if actual contains expected</t>
-  </si>
-  <si>
-    <t>Pass if actual contains expected</t>
-  </si>
-  <si>
-    <t>domain/(rest of url)</t>
-  </si>
-  <si>
-    <t>domain is homeURL specified in config file. Use to mitigate environmental differences</t>
-  </si>
-  <si>
     <t>current page url</t>
   </si>
   <si>
@@ -700,21 +667,12 @@
     <t>Yes if expecting selected. No if not.</t>
   </si>
   <si>
-    <t>Use this to handle clicks that open new tabs. New tab will be closed at the end of this check.</t>
-  </si>
-  <si>
     <t>number of pixels to scroll by</t>
   </si>
   <si>
     <t>Only used for verical scrolling</t>
   </si>
   <si>
-    <t>expected text value</t>
-  </si>
-  <si>
-    <t>Used for all text. Not just visible. Run time is slower than regular compare text</t>
-  </si>
-  <si>
     <t>url you want to navigate to</t>
   </si>
   <si>
@@ -797,9 +755,6 @@
   </si>
   <si>
     <t xml:space="preserve"> </t>
-  </si>
-  <si>
-    <t>Uses jsoup to retrieve element. Use when compare link cannot find an element that exists. Please use css selector</t>
   </si>
   <si>
     <t>decimal number</t>
@@ -1066,9 +1021,6 @@
     <t>expected url contains this text</t>
   </si>
   <si>
-    <t>Use this to handle clicks that open new tabs. New tab will be closed at the end of this check. Will check that new tab's url contains given text</t>
-  </si>
-  <si>
     <t>switch to frame</t>
   </si>
   <si>
@@ -1093,9 +1045,6 @@
     <t>Submit the form if element is a form element</t>
   </si>
   <si>
-    <t>compare current url custom</t>
-  </si>
-  <si>
     <t>compare current url contains</t>
   </si>
   <si>
@@ -1109,6 +1058,39 @@
   </si>
   <si>
     <t>VISIBLE TEXT ONLY. Check that text contains expected value</t>
+  </si>
+  <si>
+    <t>compare inner html jsoup</t>
+  </si>
+  <si>
+    <t>compare text formatted</t>
+  </si>
+  <si>
+    <t>Expected value of N/A when element has no link. Supports relative urls (start with either /, ./, or domain/).</t>
+  </si>
+  <si>
+    <t>VISIBLE TEXT ONLY.</t>
+  </si>
+  <si>
+    <t>VISIBLE TEXT ONLY.  Removes &amp;nbsp;, leading and trailing spaces, and 1 trailing new line character</t>
+  </si>
+  <si>
+    <t>Pass if actual contains expected. For HTML attributes</t>
+  </si>
+  <si>
+    <t>Pass if actual contains expected. For css values</t>
+  </si>
+  <si>
+    <t>Use this to handle clicks that open new tabs. New tab will be closed at the end of this check. Supports relative urls (start with either /, ./, or domain/).</t>
+  </si>
+  <si>
+    <t>Use this to handle clicks that open new tabs. New tab will be closed at the end of this check. Will check that new tab's url contains given text. Supports relative urls (start with either /, ./, or domain/).</t>
+  </si>
+  <si>
+    <t>Supports relative urls (start with either /, ./, or domain/).</t>
+  </si>
+  <si>
+    <t>Uses jsoup to retrieve element. Use when compare link cannot find an element that exists. Please use css selector. Supports relative urls (start with either /, ./, or domain/).</t>
   </si>
 </sst>
 </file>
@@ -1586,8 +1568,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{EEC6C929-C42E-40EE-ACD4-C5CF696595EB}" name="Table2" displayName="Table2" ref="A1:C92" totalsRowShown="0" headerRowDxfId="6" headerRowBorderDxfId="5" tableBorderDxfId="4" totalsRowBorderDxfId="3">
-  <autoFilter ref="A1:C92" xr:uid="{3A8196F3-CE1F-4FAC-85FE-2F51495F7BFB}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{EEC6C929-C42E-40EE-ACD4-C5CF696595EB}" name="Table2" displayName="Table2" ref="A1:C89" totalsRowShown="0" headerRowDxfId="6" headerRowBorderDxfId="5" tableBorderDxfId="4" totalsRowBorderDxfId="3">
+  <autoFilter ref="A1:C89" xr:uid="{3A8196F3-CE1F-4FAC-85FE-2F51495F7BFB}"/>
   <tableColumns count="3">
     <tableColumn id="1" xr3:uid="{44C580A7-5B9F-4D42-AD3F-632EC8723878}" name="Action / Keyword" dataDxfId="2"/>
     <tableColumn id="2" xr3:uid="{419EB3E1-9F00-49BC-9078-7F878531B4EC}" name="Expected" dataDxfId="1"/>
@@ -1802,7 +1784,7 @@
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C9" sqref="C9"/>
+      <selection pane="bottomLeft" activeCell="AA17" sqref="AA17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -1844,175 +1826,175 @@
       <c r="B2" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="C2" s="2" t="s">
+      <c r="C2" s="9" t="s">
+        <v>230</v>
+      </c>
+      <c r="D2" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="D2" s="2" t="s">
+      <c r="E2" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="E2" s="2" t="s">
+      <c r="F2" s="3" t="s">
         <v>10</v>
-      </c>
-      <c r="F2" s="3" t="s">
-        <v>11</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A3" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="B3" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="B3" s="1" t="s">
+      <c r="C3" s="9" t="s">
+        <v>233</v>
+      </c>
+      <c r="D3" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="C3" s="1" t="s">
+      <c r="E3" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="D3" s="1" t="s">
+      <c r="F3" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="E3" s="4" t="s">
+      <c r="H3" s="5"/>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A4" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="F3" s="3" t="s">
+      <c r="B4" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="H3" s="5"/>
-    </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A4" s="1" t="s">
+      <c r="C4" s="9" t="s">
         <v>18</v>
       </c>
-      <c r="B4" s="1" t="s">
+      <c r="D4" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="C4" s="9" t="s">
-        <v>246</v>
-      </c>
-      <c r="D4" s="1" t="s">
+      <c r="E4" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="F4" s="3" t="s">
         <v>21</v>
-      </c>
-      <c r="E4" s="4" t="s">
-        <v>22</v>
-      </c>
-      <c r="F4" s="3" t="s">
-        <v>23</v>
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A5" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="C5" s="9" t="s">
         <v>24</v>
       </c>
-      <c r="B5" s="1" t="s">
+      <c r="D5" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="C5" s="9" t="s">
-        <v>247</v>
-      </c>
-      <c r="D5" s="1" t="s">
+      <c r="E5" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="F5" s="3" t="s">
         <v>27</v>
-      </c>
-      <c r="E5" s="4" t="s">
-        <v>28</v>
-      </c>
-      <c r="F5" s="3" t="s">
-        <v>29</v>
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A6" s="1" t="s">
-        <v>30</v>
+        <v>236</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="C6" s="9" t="s">
-        <v>20</v>
+        <v>235</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="E6" s="6"/>
       <c r="F6" s="7"/>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A7" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="B7" s="8" t="s">
+        <v>219</v>
+      </c>
+      <c r="C7" s="9"/>
+      <c r="D7" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="E7" s="4" t="s">
         <v>33</v>
       </c>
-      <c r="B7" s="8" t="s">
-        <v>234</v>
-      </c>
-      <c r="C7" s="9" t="s">
-        <v>26</v>
-      </c>
-      <c r="D7" s="1" t="s">
-        <v>35</v>
-      </c>
-      <c r="E7" s="4" t="s">
-        <v>36</v>
-      </c>
       <c r="F7" s="9" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="H7" s="5"/>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A8" s="1"/>
       <c r="C8" s="9" t="s">
-        <v>250</v>
+        <v>31</v>
       </c>
       <c r="D8" s="1" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="E8" s="4" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="F8" s="1" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A9" s="8"/>
       <c r="B9" s="1" t="s">
-        <v>38</v>
-      </c>
-      <c r="C9" s="9"/>
+        <v>35</v>
+      </c>
+      <c r="C9" s="9" t="s">
+        <v>36</v>
+      </c>
       <c r="D9" s="8"/>
       <c r="E9" s="4" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="F9" s="3" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A10" s="8"/>
       <c r="B10" s="1" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="C10" s="9" t="s">
-        <v>34</v>
+        <v>41</v>
       </c>
       <c r="D10" s="1" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="E10" s="6"/>
       <c r="F10" s="3" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A11" s="8"/>
       <c r="B11" s="1" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="C11" s="9" t="s">
-        <v>39</v>
+        <v>45</v>
       </c>
       <c r="D11" s="1" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
       <c r="E11" s="4" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="F11" s="7"/>
       <c r="H11" s="5"/>
@@ -2021,29 +2003,27 @@
       <c r="A12" s="8"/>
       <c r="B12" s="8"/>
       <c r="C12" s="9" t="s">
-        <v>44</v>
+        <v>48</v>
       </c>
       <c r="D12" s="3" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="E12" s="4" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="F12" s="7"/>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A13" s="8"/>
       <c r="B13" s="1" t="s">
-        <v>54</v>
-      </c>
-      <c r="C13" s="9" t="s">
-        <v>48</v>
-      </c>
+        <v>51</v>
+      </c>
+      <c r="C13" s="9"/>
       <c r="D13" s="3" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
       <c r="E13" s="4" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="F13" s="7"/>
       <c r="H13" s="5"/>
@@ -2051,28 +2031,30 @@
     <row r="14" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A14" s="8"/>
       <c r="B14" s="1" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="C14" s="9" t="s">
-        <v>51</v>
+        <v>55</v>
       </c>
       <c r="D14" s="3" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="E14" s="4" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
       <c r="F14" s="7"/>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A15" s="8"/>
       <c r="B15" s="8"/>
-      <c r="C15" s="9"/>
+      <c r="C15" s="9" t="s">
+        <v>58</v>
+      </c>
       <c r="D15" s="3" t="s">
-        <v>66</v>
+        <v>62</v>
       </c>
       <c r="E15" s="4" t="s">
-        <v>67</v>
+        <v>63</v>
       </c>
       <c r="F15" s="7"/>
       <c r="H15" s="5"/>
@@ -2080,13 +2062,10 @@
     <row r="16" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A16" s="8"/>
       <c r="B16" s="1" t="s">
-        <v>64</v>
-      </c>
-      <c r="C16" s="9" t="s">
-        <v>58</v>
+        <v>61</v>
       </c>
       <c r="D16" s="3" t="s">
-        <v>69</v>
+        <v>65</v>
       </c>
       <c r="E16" s="6"/>
       <c r="F16" s="7"/>
@@ -2094,81 +2073,79 @@
     <row r="17" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A17" s="8"/>
       <c r="B17" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="C17" s="9" t="s">
+        <v>67</v>
+      </c>
+      <c r="D17" s="3" t="s">
         <v>68</v>
       </c>
-      <c r="C17" s="9" t="s">
-        <v>61</v>
-      </c>
-      <c r="D17" s="3" t="s">
-        <v>72</v>
-      </c>
       <c r="E17" s="4" t="s">
-        <v>73</v>
+        <v>69</v>
       </c>
       <c r="F17" s="7"/>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A18" s="8"/>
       <c r="B18" s="1" t="s">
-        <v>70</v>
+        <v>66</v>
       </c>
       <c r="C18" s="9" t="s">
-        <v>65</v>
+        <v>71</v>
       </c>
       <c r="E18" s="4" t="s">
-        <v>235</v>
+        <v>220</v>
       </c>
       <c r="F18" s="7"/>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A19" s="8"/>
       <c r="B19" s="1" t="s">
-        <v>74</v>
-      </c>
-      <c r="C19" s="15"/>
+        <v>70</v>
+      </c>
+      <c r="C19" s="9" t="s">
+        <v>72</v>
+      </c>
       <c r="D19" s="2" t="s">
-        <v>77</v>
+        <v>73</v>
       </c>
       <c r="F19" s="7"/>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A20" s="12"/>
       <c r="B20" s="12"/>
-      <c r="C20" s="9" t="s">
-        <v>71</v>
+      <c r="C20" s="11" t="s">
+        <v>75</v>
       </c>
       <c r="D20" s="11" t="s">
-        <v>80</v>
+        <v>76</v>
       </c>
       <c r="E20" s="11" t="s">
-        <v>78</v>
+        <v>74</v>
       </c>
       <c r="F20" s="12"/>
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A21" s="7"/>
       <c r="B21" s="15" t="s">
-        <v>238</v>
-      </c>
-      <c r="C21" s="9" t="s">
-        <v>75</v>
-      </c>
+        <v>222</v>
+      </c>
+      <c r="C21" s="11"/>
       <c r="D21" s="13"/>
       <c r="E21" s="11" t="s">
-        <v>81</v>
+        <v>77</v>
       </c>
       <c r="F21" s="7"/>
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A22" s="7"/>
       <c r="B22" s="15" t="s">
-        <v>240</v>
-      </c>
-      <c r="C22" s="9" t="s">
-        <v>76</v>
-      </c>
+        <v>224</v>
+      </c>
+      <c r="C22" s="7"/>
       <c r="D22" s="11" t="s">
-        <v>82</v>
+        <v>78</v>
       </c>
       <c r="E22" s="13"/>
       <c r="F22" s="7"/>
@@ -2176,28 +2153,26 @@
     <row r="23" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A23" s="7"/>
       <c r="B23" s="7"/>
-      <c r="C23" s="11" t="s">
+      <c r="C23" s="7"/>
+      <c r="D23" s="11" t="s">
+        <v>80</v>
+      </c>
+      <c r="E23" s="14" t="s">
         <v>79</v>
-      </c>
-      <c r="D23" s="11" t="s">
-        <v>84</v>
-      </c>
-      <c r="E23" s="14" t="s">
-        <v>83</v>
       </c>
       <c r="F23" s="7"/>
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A24" s="7"/>
       <c r="B24" s="15" t="s">
-        <v>244</v>
+        <v>228</v>
       </c>
       <c r="C24" s="7"/>
       <c r="D24" s="11" t="s">
-        <v>86</v>
+        <v>82</v>
       </c>
       <c r="E24" s="11" t="s">
-        <v>85</v>
+        <v>81</v>
       </c>
       <c r="F24" s="7"/>
     </row>
@@ -2206,10 +2181,10 @@
       <c r="B25" s="7"/>
       <c r="C25" s="7"/>
       <c r="D25" s="11" t="s">
-        <v>88</v>
+        <v>84</v>
       </c>
       <c r="E25" s="11" t="s">
-        <v>87</v>
+        <v>83</v>
       </c>
       <c r="F25" s="7"/>
     </row>
@@ -2226,164 +2201,164 @@
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:Y92"/>
+  <dimension ref="A1:Y89"/>
   <sheetViews>
-    <sheetView showGridLines="0" topLeftCell="B1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C8" sqref="C8"/>
+    <sheetView showGridLines="0" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A79" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B91" sqref="B91"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="29.28515625" customWidth="1"/>
     <col min="2" max="2" width="39.85546875" customWidth="1"/>
-    <col min="3" max="3" width="137.28515625" customWidth="1"/>
+    <col min="3" max="3" width="169.85546875" bestFit="1" customWidth="1"/>
     <col min="5" max="25" width="14.42578125" hidden="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A1" s="37" t="s">
-        <v>89</v>
+        <v>85</v>
       </c>
       <c r="B1" s="38" t="s">
-        <v>90</v>
+        <v>86</v>
       </c>
       <c r="C1" s="39" t="s">
-        <v>91</v>
+        <v>87</v>
       </c>
     </row>
     <row r="2" spans="1:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A2" s="26" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="B2" s="11" t="s">
-        <v>92</v>
+        <v>88</v>
       </c>
       <c r="C2" s="6" t="s">
-        <v>93</v>
+        <v>237</v>
       </c>
     </row>
     <row r="3" spans="1:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A3" s="26" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B3" s="11" t="s">
-        <v>94</v>
+        <v>89</v>
       </c>
       <c r="C3" s="6" t="s">
-        <v>95</v>
+        <v>238</v>
       </c>
     </row>
     <row r="4" spans="1:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A4" s="26" t="s">
-        <v>77</v>
+        <v>73</v>
       </c>
       <c r="B4" s="11" t="s">
-        <v>96</v>
+        <v>90</v>
       </c>
       <c r="C4" s="6" t="s">
-        <v>97</v>
+        <v>91</v>
       </c>
     </row>
     <row r="5" spans="1:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A5" s="26" t="s">
-        <v>83</v>
+        <v>79</v>
       </c>
       <c r="B5" s="11" t="s">
-        <v>98</v>
+        <v>92</v>
       </c>
       <c r="C5" s="6" t="s">
-        <v>99</v>
+        <v>93</v>
       </c>
     </row>
     <row r="6" spans="1:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A6" s="26" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B6" s="11" t="s">
-        <v>98</v>
+        <v>92</v>
       </c>
       <c r="C6" s="6" t="s">
-        <v>242</v>
+        <v>226</v>
       </c>
     </row>
     <row r="7" spans="1:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A7" s="26" t="s">
-        <v>30</v>
+        <v>236</v>
       </c>
       <c r="B7" s="11" t="s">
-        <v>94</v>
+        <v>89</v>
       </c>
       <c r="C7" s="6" t="s">
-        <v>100</v>
+        <v>239</v>
       </c>
     </row>
     <row r="8" spans="1:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A8" s="26" t="s">
-        <v>250</v>
+        <v>233</v>
       </c>
       <c r="B8" s="11" t="s">
-        <v>94</v>
+        <v>89</v>
       </c>
       <c r="C8" s="6" t="s">
-        <v>251</v>
+        <v>234</v>
       </c>
     </row>
     <row r="9" spans="1:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A9" s="26" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="B9" s="11" t="s">
-        <v>101</v>
+        <v>94</v>
       </c>
       <c r="C9" s="30" t="s">
-        <v>102</v>
+        <v>95</v>
       </c>
     </row>
     <row r="10" spans="1:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A10" s="27" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="B10" s="11" t="s">
-        <v>103</v>
+        <v>96</v>
       </c>
       <c r="C10" s="4"/>
     </row>
     <row r="11" spans="1:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A11" s="27" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="B11" s="11" t="s">
-        <v>103</v>
+        <v>96</v>
       </c>
       <c r="C11" s="4"/>
     </row>
     <row r="12" spans="1:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A12" s="26" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="B12" s="11" t="s">
-        <v>101</v>
+        <v>94</v>
       </c>
       <c r="C12" s="6" t="s">
-        <v>102</v>
+        <v>95</v>
       </c>
     </row>
     <row r="13" spans="1:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A13" s="27" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="B13" s="11" t="s">
-        <v>103</v>
+        <v>96</v>
       </c>
       <c r="C13" s="4"/>
     </row>
     <row r="14" spans="1:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A14" s="27" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="B14" s="11" t="s">
-        <v>103</v>
+        <v>96</v>
       </c>
       <c r="C14" s="4"/>
     </row>
@@ -2392,19 +2367,19 @@
         <v>7</v>
       </c>
       <c r="B15" s="11" t="s">
-        <v>104</v>
+        <v>97</v>
       </c>
       <c r="C15" s="6"/>
     </row>
     <row r="16" spans="1:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A16" s="26" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B16" s="15" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C16" s="6" t="s">
-        <v>105</v>
+        <v>98</v>
       </c>
     </row>
     <row r="17" spans="1:3" ht="12.75" x14ac:dyDescent="0.2">
@@ -2412,673 +2387,675 @@
         <v>6</v>
       </c>
       <c r="B17" s="11" t="s">
-        <v>106</v>
+        <v>99</v>
       </c>
       <c r="C17" s="6"/>
     </row>
     <row r="18" spans="1:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A18" s="28" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="B18" s="16" t="s">
-        <v>107</v>
+        <v>100</v>
       </c>
       <c r="C18" s="31"/>
     </row>
     <row r="19" spans="1:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A19" s="28" t="s">
-        <v>108</v>
+        <v>101</v>
       </c>
       <c r="B19" s="16" t="s">
-        <v>109</v>
+        <v>102</v>
       </c>
       <c r="C19" s="31"/>
     </row>
     <row r="20" spans="1:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A20" s="28" t="s">
-        <v>110</v>
+        <v>103</v>
       </c>
       <c r="B20" s="18" t="s">
-        <v>111</v>
-      </c>
-      <c r="C20" s="31" t="s">
-        <v>112</v>
+        <v>104</v>
+      </c>
+      <c r="C20" s="4" t="s">
+        <v>240</v>
       </c>
     </row>
     <row r="21" spans="1:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A21" s="28" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="B21" s="18" t="s">
-        <v>111</v>
-      </c>
-      <c r="C21" s="31" t="s">
-        <v>113</v>
+        <v>104</v>
+      </c>
+      <c r="C21" s="4" t="s">
+        <v>241</v>
       </c>
     </row>
     <row r="22" spans="1:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A22" s="26" t="s">
-        <v>8</v>
+        <v>22</v>
       </c>
       <c r="B22" s="15" t="s">
-        <v>114</v>
-      </c>
-      <c r="C22" s="6" t="s">
-        <v>115</v>
-      </c>
+        <v>105</v>
+      </c>
+      <c r="C22" s="6"/>
     </row>
     <row r="23" spans="1:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A23" s="26" t="s">
-        <v>24</v>
-      </c>
-      <c r="B23" s="15" t="s">
-        <v>116</v>
-      </c>
-      <c r="C23" s="6"/>
+        <v>67</v>
+      </c>
+      <c r="B23" s="11" t="s">
+        <v>106</v>
+      </c>
+      <c r="C23" s="6" t="s">
+        <v>107</v>
+      </c>
     </row>
     <row r="24" spans="1:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A24" s="26" t="s">
         <v>71</v>
       </c>
       <c r="B24" s="11" t="s">
-        <v>117</v>
+        <v>106</v>
       </c>
       <c r="C24" s="6" t="s">
-        <v>118</v>
+        <v>108</v>
       </c>
     </row>
     <row r="25" spans="1:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A25" s="26" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
       <c r="B25" s="11" t="s">
-        <v>117</v>
+        <v>106</v>
       </c>
       <c r="C25" s="6" t="s">
-        <v>119</v>
+        <v>109</v>
       </c>
     </row>
     <row r="26" spans="1:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A26" s="26" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="B26" s="11" t="s">
-        <v>117</v>
+        <v>106</v>
       </c>
       <c r="C26" s="6" t="s">
-        <v>120</v>
+        <v>110</v>
       </c>
     </row>
     <row r="27" spans="1:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A27" s="26" t="s">
-        <v>79</v>
+        <v>28</v>
       </c>
       <c r="B27" s="11" t="s">
-        <v>117</v>
-      </c>
-      <c r="C27" s="6" t="s">
-        <v>121</v>
-      </c>
+        <v>111</v>
+      </c>
+      <c r="C27" s="6"/>
     </row>
     <row r="28" spans="1:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A28" s="26" t="s">
-        <v>31</v>
-      </c>
-      <c r="B28" s="11" t="s">
-        <v>122</v>
-      </c>
-      <c r="C28" s="6"/>
+        <v>23</v>
+      </c>
+      <c r="B28" s="8"/>
+      <c r="C28" s="6" t="s">
+        <v>112</v>
+      </c>
     </row>
     <row r="29" spans="1:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A29" s="26" t="s">
-        <v>25</v>
-      </c>
-      <c r="B29" s="8"/>
-      <c r="C29" s="6" t="s">
-        <v>123</v>
-      </c>
+        <v>35</v>
+      </c>
+      <c r="B29" s="11" t="s">
+        <v>113</v>
+      </c>
+      <c r="C29" s="6"/>
     </row>
     <row r="30" spans="1:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A30" s="26" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="B30" s="11" t="s">
-        <v>124</v>
-      </c>
-      <c r="C30" s="6"/>
+        <v>114</v>
+      </c>
+      <c r="C30" s="6" t="s">
+        <v>115</v>
+      </c>
     </row>
     <row r="31" spans="1:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A31" s="26" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="B31" s="11" t="s">
-        <v>125</v>
+        <v>116</v>
       </c>
       <c r="C31" s="6" t="s">
-        <v>126</v>
+        <v>117</v>
       </c>
     </row>
     <row r="32" spans="1:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A32" s="26" t="s">
-        <v>47</v>
+        <v>76</v>
       </c>
       <c r="B32" s="11" t="s">
-        <v>127</v>
+        <v>90</v>
       </c>
       <c r="C32" s="6" t="s">
-        <v>128</v>
+        <v>118</v>
       </c>
     </row>
     <row r="33" spans="1:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A33" s="26" t="s">
-        <v>80</v>
+        <v>69</v>
       </c>
       <c r="B33" s="11" t="s">
-        <v>96</v>
+        <v>88</v>
       </c>
       <c r="C33" s="6" t="s">
-        <v>129</v>
+        <v>242</v>
       </c>
     </row>
     <row r="34" spans="1:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A34" s="26" t="s">
-        <v>73</v>
+        <v>220</v>
       </c>
       <c r="B34" s="11" t="s">
-        <v>92</v>
+        <v>221</v>
       </c>
       <c r="C34" s="6" t="s">
-        <v>130</v>
+        <v>243</v>
       </c>
     </row>
     <row r="35" spans="1:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A35" s="26" t="s">
-        <v>235</v>
+        <v>81</v>
       </c>
       <c r="B35" s="11" t="s">
-        <v>236</v>
-      </c>
-      <c r="C35" s="6" t="s">
-        <v>237</v>
+        <v>119</v>
+      </c>
+      <c r="C35" s="30" t="s">
+        <v>120</v>
       </c>
     </row>
     <row r="36" spans="1:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A36" s="26" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="B36" s="11" t="s">
-        <v>131</v>
-      </c>
-      <c r="C36" s="30" t="s">
-        <v>132</v>
-      </c>
+        <v>92</v>
+      </c>
+      <c r="C36" s="6"/>
     </row>
     <row r="37" spans="1:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A37" s="26" t="s">
-        <v>87</v>
+        <v>17</v>
       </c>
       <c r="B37" s="11" t="s">
-        <v>98</v>
-      </c>
-      <c r="C37" s="6"/>
+        <v>121</v>
+      </c>
+      <c r="C37" s="6" t="s">
+        <v>244</v>
+      </c>
     </row>
     <row r="38" spans="1:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A38" s="26" t="s">
-        <v>14</v>
-      </c>
-      <c r="B38" s="11" t="s">
-        <v>133</v>
-      </c>
+        <v>74</v>
+      </c>
+      <c r="B38" s="8"/>
       <c r="C38" s="6" t="s">
-        <v>134</v>
+        <v>122</v>
       </c>
     </row>
     <row r="39" spans="1:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A39" s="26" t="s">
-        <v>19</v>
-      </c>
-      <c r="B39" s="11" t="s">
-        <v>135</v>
-      </c>
-      <c r="C39" s="6"/>
+        <v>77</v>
+      </c>
+      <c r="B39" s="15" t="s">
+        <v>94</v>
+      </c>
+      <c r="C39" s="6" t="s">
+        <v>123</v>
+      </c>
     </row>
     <row r="40" spans="1:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A40" s="26" t="s">
-        <v>78</v>
+        <v>33</v>
       </c>
       <c r="B40" s="8"/>
       <c r="C40" s="6" t="s">
-        <v>136</v>
+        <v>124</v>
       </c>
     </row>
     <row r="41" spans="1:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A41" s="26" t="s">
-        <v>81</v>
-      </c>
-      <c r="B41" s="15" t="s">
-        <v>101</v>
-      </c>
+        <v>14</v>
+      </c>
+      <c r="B41" s="8"/>
       <c r="C41" s="6" t="s">
-        <v>137</v>
+        <v>227</v>
       </c>
     </row>
     <row r="42" spans="1:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A42" s="26" t="s">
-        <v>36</v>
+        <v>38</v>
       </c>
       <c r="B42" s="8"/>
       <c r="C42" s="6" t="s">
-        <v>138</v>
+        <v>125</v>
       </c>
     </row>
     <row r="43" spans="1:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A43" s="26" t="s">
-        <v>16</v>
+        <v>20</v>
       </c>
       <c r="B43" s="8"/>
-      <c r="C43" s="6" t="s">
-        <v>243</v>
-      </c>
+      <c r="C43" s="6"/>
     </row>
     <row r="44" spans="1:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A44" s="26" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="B44" s="8"/>
       <c r="C44" s="6" t="s">
-        <v>139</v>
+        <v>126</v>
       </c>
     </row>
     <row r="45" spans="1:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A45" s="26" t="s">
-        <v>22</v>
+        <v>26</v>
       </c>
       <c r="B45" s="8"/>
       <c r="C45" s="6"/>
     </row>
     <row r="46" spans="1:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A46" s="26" t="s">
-        <v>45</v>
+        <v>57</v>
       </c>
       <c r="B46" s="8"/>
       <c r="C46" s="6" t="s">
-        <v>140</v>
+        <v>127</v>
       </c>
     </row>
     <row r="47" spans="1:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A47" s="26" t="s">
-        <v>28</v>
+        <v>60</v>
       </c>
       <c r="B47" s="8"/>
-      <c r="C47" s="6"/>
+      <c r="C47" s="6" t="s">
+        <v>128</v>
+      </c>
     </row>
     <row r="48" spans="1:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A48" s="26" t="s">
-        <v>60</v>
+        <v>50</v>
       </c>
       <c r="B48" s="8"/>
       <c r="C48" s="6" t="s">
-        <v>141</v>
+        <v>129</v>
       </c>
     </row>
     <row r="49" spans="1:4" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A49" s="26" t="s">
-        <v>63</v>
+        <v>53</v>
       </c>
       <c r="B49" s="8"/>
       <c r="C49" s="6" t="s">
-        <v>142</v>
+        <v>130</v>
       </c>
     </row>
     <row r="50" spans="1:4" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A50" s="26" t="s">
-        <v>53</v>
-      </c>
-      <c r="B50" s="8"/>
+        <v>54</v>
+      </c>
+      <c r="B50" s="11" t="s">
+        <v>106</v>
+      </c>
       <c r="C50" s="6" t="s">
-        <v>143</v>
+        <v>131</v>
       </c>
     </row>
     <row r="51" spans="1:4" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A51" s="26" t="s">
-        <v>56</v>
-      </c>
-      <c r="B51" s="8"/>
+        <v>51</v>
+      </c>
+      <c r="B51" s="15" t="s">
+        <v>94</v>
+      </c>
       <c r="C51" s="6" t="s">
-        <v>144</v>
+        <v>132</v>
       </c>
     </row>
     <row r="52" spans="1:4" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A52" s="26" t="s">
-        <v>57</v>
+        <v>63</v>
       </c>
       <c r="B52" s="11" t="s">
-        <v>117</v>
-      </c>
-      <c r="C52" s="6" t="s">
-        <v>145</v>
+        <v>133</v>
+      </c>
+      <c r="C52" s="30" t="s">
+        <v>134</v>
       </c>
     </row>
     <row r="53" spans="1:4" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A53" s="26" t="s">
-        <v>54</v>
+        <v>31</v>
       </c>
       <c r="B53" s="15" t="s">
-        <v>101</v>
+        <v>135</v>
       </c>
       <c r="C53" s="6" t="s">
-        <v>146</v>
+        <v>136</v>
       </c>
     </row>
     <row r="54" spans="1:4" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A54" s="26" t="s">
-        <v>67</v>
+        <v>36</v>
       </c>
       <c r="B54" s="11" t="s">
-        <v>147</v>
-      </c>
-      <c r="C54" s="30" t="s">
-        <v>148</v>
+        <v>106</v>
+      </c>
+      <c r="C54" s="6" t="s">
+        <v>137</v>
       </c>
     </row>
     <row r="55" spans="1:4" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A55" s="26" t="s">
-        <v>34</v>
+        <v>41</v>
       </c>
       <c r="B55" s="15" t="s">
-        <v>149</v>
+        <v>138</v>
       </c>
       <c r="C55" s="6" t="s">
-        <v>150</v>
+        <v>139</v>
       </c>
     </row>
     <row r="56" spans="1:4" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A56" s="26" t="s">
-        <v>39</v>
+        <v>45</v>
       </c>
       <c r="B56" s="11" t="s">
-        <v>117</v>
+        <v>106</v>
       </c>
       <c r="C56" s="6" t="s">
-        <v>151</v>
+        <v>140</v>
       </c>
     </row>
     <row r="57" spans="1:4" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A57" s="26" t="s">
-        <v>44</v>
-      </c>
-      <c r="B57" s="15" t="s">
-        <v>152</v>
+        <v>48</v>
+      </c>
+      <c r="B57" s="11" t="s">
+        <v>106</v>
       </c>
       <c r="C57" s="6" t="s">
-        <v>153</v>
+        <v>141</v>
       </c>
     </row>
     <row r="58" spans="1:4" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A58" s="26" t="s">
-        <v>48</v>
-      </c>
-      <c r="B58" s="11" t="s">
-        <v>117</v>
-      </c>
+        <v>235</v>
+      </c>
+      <c r="B58" s="15"/>
       <c r="C58" s="6" t="s">
-        <v>154</v>
+        <v>142</v>
       </c>
     </row>
     <row r="59" spans="1:4" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A59" s="26" t="s">
-        <v>51</v>
-      </c>
-      <c r="B59" s="11" t="s">
-        <v>117</v>
-      </c>
-      <c r="C59" s="6" t="s">
-        <v>155</v>
+      <c r="A59" s="27" t="s">
+        <v>34</v>
+      </c>
+      <c r="B59" s="8"/>
+      <c r="C59" s="4" t="s">
+        <v>143</v>
       </c>
     </row>
     <row r="60" spans="1:4" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A60" s="26" t="s">
-        <v>65</v>
-      </c>
-      <c r="B60" s="15"/>
-      <c r="C60" s="6" t="s">
-        <v>156</v>
+      <c r="A60" s="27" t="s">
+        <v>39</v>
+      </c>
+      <c r="B60" s="8"/>
+      <c r="C60" s="4" t="s">
+        <v>144</v>
       </c>
     </row>
     <row r="61" spans="1:4" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A61" s="27" t="s">
-        <v>37</v>
-      </c>
-      <c r="B61" s="8"/>
-      <c r="C61" s="4" t="s">
-        <v>157</v>
+      <c r="A61" s="28" t="s">
+        <v>43</v>
+      </c>
+      <c r="B61" s="7"/>
+      <c r="C61" s="31" t="s">
+        <v>145</v>
       </c>
     </row>
     <row r="62" spans="1:4" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A62" s="27" t="s">
-        <v>42</v>
-      </c>
-      <c r="B62" s="8"/>
-      <c r="C62" s="4" t="s">
-        <v>158</v>
+      <c r="A62" s="28" t="s">
+        <v>47</v>
+      </c>
+      <c r="B62" s="7"/>
+      <c r="C62" s="31" t="s">
+        <v>146</v>
+      </c>
+      <c r="D62" s="19" t="s">
+        <v>148</v>
       </c>
     </row>
     <row r="63" spans="1:4" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A63" s="28" t="s">
-        <v>46</v>
+        <v>24</v>
       </c>
       <c r="B63" s="7"/>
       <c r="C63" s="31" t="s">
-        <v>159</v>
+        <v>147</v>
+      </c>
+      <c r="D63" s="19" t="s">
+        <v>148</v>
       </c>
     </row>
     <row r="64" spans="1:4" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A64" s="28" t="s">
-        <v>50</v>
+        <v>18</v>
       </c>
       <c r="B64" s="7"/>
-      <c r="C64" s="31" t="s">
+      <c r="C64" s="4" t="s">
+        <v>245</v>
+      </c>
+    </row>
+    <row r="65" spans="1:3" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A65" s="27" t="s">
+        <v>46</v>
+      </c>
+      <c r="B65" s="20" t="s">
+        <v>149</v>
+      </c>
+      <c r="C65" s="31" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="66" spans="1:3" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A66" s="27" t="s">
+        <v>49</v>
+      </c>
+      <c r="B66" s="20" t="s">
+        <v>149</v>
+      </c>
+      <c r="C66" s="31" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="67" spans="1:3" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A67" s="28" t="s">
+        <v>52</v>
+      </c>
+      <c r="B67" s="20" t="s">
+        <v>149</v>
+      </c>
+      <c r="C67" s="31" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="68" spans="1:3" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A68" s="28" t="s">
+        <v>56</v>
+      </c>
+      <c r="B68" s="20" t="s">
+        <v>149</v>
+      </c>
+      <c r="C68" s="31" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="69" spans="1:3" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A69" s="28" t="s">
+        <v>59</v>
+      </c>
+      <c r="B69" s="20" t="s">
+        <v>149</v>
+      </c>
+      <c r="C69" s="31" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="70" spans="1:3" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A70" s="28" t="s">
+        <v>62</v>
+      </c>
+      <c r="B70" s="20" t="s">
+        <v>149</v>
+      </c>
+      <c r="C70" s="31" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="71" spans="1:3" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A71" s="28" t="s">
+        <v>65</v>
+      </c>
+      <c r="B71" s="20" t="s">
+        <v>149</v>
+      </c>
+      <c r="C71" s="31" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="72" spans="1:3" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A72" s="28" t="s">
+        <v>68</v>
+      </c>
+      <c r="B72" s="20" t="s">
+        <v>149</v>
+      </c>
+      <c r="C72" s="31" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="73" spans="1:3" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A73" s="28" t="s">
+        <v>64</v>
+      </c>
+      <c r="B73" s="20" t="s">
+        <v>158</v>
+      </c>
+      <c r="C73" s="32" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="74" spans="1:3" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A74" s="28" t="s">
+        <v>61</v>
+      </c>
+      <c r="B74" s="20" t="s">
         <v>160</v>
       </c>
-      <c r="D64" s="19" t="s">
+      <c r="C74" s="32" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="75" spans="1:3" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A75" s="28" t="s">
+        <v>66</v>
+      </c>
+      <c r="B75" s="20" t="s">
         <v>162</v>
       </c>
-    </row>
-    <row r="65" spans="1:4" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A65" s="28" t="s">
-        <v>26</v>
-      </c>
-      <c r="B65" s="7"/>
-      <c r="C65" s="31" t="s">
-        <v>161</v>
-      </c>
-      <c r="D65" s="19" t="s">
-        <v>162</v>
-      </c>
-    </row>
-    <row r="66" spans="1:4" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A66" s="28" t="s">
-        <v>20</v>
-      </c>
-      <c r="B66" s="7"/>
-      <c r="C66" s="31" t="s">
+      <c r="C75" s="31" t="s">
         <v>163</v>
       </c>
     </row>
-    <row r="67" spans="1:4" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A67" s="27" t="s">
-        <v>49</v>
-      </c>
-      <c r="B67" s="20" t="s">
+    <row r="76" spans="1:3" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A76" s="28" t="s">
+        <v>70</v>
+      </c>
+      <c r="B76" s="20" t="s">
         <v>164</v>
       </c>
-      <c r="C67" s="31" t="s">
+      <c r="C76" s="32" t="s">
         <v>165</v>
       </c>
     </row>
-    <row r="68" spans="1:4" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A68" s="27" t="s">
-        <v>52</v>
-      </c>
-      <c r="B68" s="20" t="s">
-        <v>164</v>
-      </c>
-      <c r="C68" s="31" t="s">
+    <row r="77" spans="1:3" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A77" s="28" t="s">
+        <v>10</v>
+      </c>
+      <c r="B77" s="20" t="s">
         <v>166</v>
       </c>
-    </row>
-    <row r="69" spans="1:4" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A69" s="28" t="s">
-        <v>55</v>
-      </c>
-      <c r="B69" s="20" t="s">
-        <v>164</v>
-      </c>
-      <c r="C69" s="31" t="s">
+      <c r="C77" s="31" t="s">
         <v>167</v>
       </c>
     </row>
-    <row r="70" spans="1:4" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A70" s="28" t="s">
-        <v>59</v>
-      </c>
-      <c r="B70" s="20" t="s">
-        <v>164</v>
-      </c>
-      <c r="C70" s="31" t="s">
+    <row r="78" spans="1:3" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A78" s="28" t="s">
+        <v>27</v>
+      </c>
+      <c r="B78" s="20" t="s">
+        <v>166</v>
+      </c>
+      <c r="C78" s="31" t="s">
         <v>168</v>
       </c>
     </row>
-    <row r="71" spans="1:4" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A71" s="28" t="s">
-        <v>62</v>
-      </c>
-      <c r="B71" s="20" t="s">
-        <v>164</v>
-      </c>
-      <c r="C71" s="31" t="s">
+    <row r="79" spans="1:3" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A79" s="28" t="s">
+        <v>15</v>
+      </c>
+      <c r="B79" s="20" t="s">
+        <v>166</v>
+      </c>
+      <c r="C79" s="31" t="s">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="80" spans="1:3" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A80" s="28" t="s">
+        <v>21</v>
+      </c>
+      <c r="B80" s="20" t="s">
+        <v>166</v>
+      </c>
+      <c r="C80" s="31" t="s">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="81" spans="1:3" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A81" s="29" t="s">
+        <v>78</v>
+      </c>
+      <c r="B81" s="20" t="s">
         <v>169</v>
       </c>
-    </row>
-    <row r="72" spans="1:4" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A72" s="28" t="s">
-        <v>66</v>
-      </c>
-      <c r="B72" s="20" t="s">
-        <v>164</v>
-      </c>
-      <c r="C72" s="31" t="s">
+      <c r="C81" s="33" t="s">
         <v>170</v>
       </c>
     </row>
-    <row r="73" spans="1:4" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A73" s="28" t="s">
-        <v>69</v>
-      </c>
-      <c r="B73" s="20" t="s">
-        <v>164</v>
-      </c>
-      <c r="C73" s="31" t="s">
+    <row r="82" spans="1:3" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A82" s="29" t="s">
+        <v>80</v>
+      </c>
+      <c r="B82" s="20" t="s">
         <v>171</v>
       </c>
-    </row>
-    <row r="74" spans="1:4" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A74" s="28" t="s">
-        <v>72</v>
-      </c>
-      <c r="B74" s="20" t="s">
-        <v>164</v>
-      </c>
-      <c r="C74" s="31" t="s">
+      <c r="C82" s="33" t="s">
         <v>172</v>
-      </c>
-    </row>
-    <row r="75" spans="1:4" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A75" s="28" t="s">
-        <v>68</v>
-      </c>
-      <c r="B75" s="20" t="s">
-        <v>173</v>
-      </c>
-      <c r="C75" s="32" t="s">
-        <v>174</v>
-      </c>
-    </row>
-    <row r="76" spans="1:4" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A76" s="28" t="s">
-        <v>64</v>
-      </c>
-      <c r="B76" s="20" t="s">
-        <v>175</v>
-      </c>
-      <c r="C76" s="32" t="s">
-        <v>176</v>
-      </c>
-    </row>
-    <row r="77" spans="1:4" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A77" s="28" t="s">
-        <v>70</v>
-      </c>
-      <c r="B77" s="20" t="s">
-        <v>177</v>
-      </c>
-      <c r="C77" s="31" t="s">
-        <v>178</v>
-      </c>
-    </row>
-    <row r="78" spans="1:4" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A78" s="28" t="s">
-        <v>74</v>
-      </c>
-      <c r="B78" s="20" t="s">
-        <v>179</v>
-      </c>
-      <c r="C78" s="32" t="s">
-        <v>180</v>
-      </c>
-    </row>
-    <row r="79" spans="1:4" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A79" s="28" t="s">
-        <v>11</v>
-      </c>
-      <c r="B79" s="20" t="s">
-        <v>181</v>
-      </c>
-      <c r="C79" s="31" t="s">
-        <v>182</v>
-      </c>
-    </row>
-    <row r="80" spans="1:4" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A80" s="28" t="s">
-        <v>29</v>
-      </c>
-      <c r="B80" s="20" t="s">
-        <v>181</v>
-      </c>
-      <c r="C80" s="31" t="s">
-        <v>183</v>
-      </c>
-    </row>
-    <row r="81" spans="1:3" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A81" s="28" t="s">
-        <v>17</v>
-      </c>
-      <c r="B81" s="20" t="s">
-        <v>181</v>
-      </c>
-      <c r="C81" s="31" t="s">
-        <v>183</v>
-      </c>
-    </row>
-    <row r="82" spans="1:3" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A82" s="28" t="s">
-        <v>23</v>
-      </c>
-      <c r="B82" s="20" t="s">
-        <v>181</v>
-      </c>
-      <c r="C82" s="31" t="s">
-        <v>183</v>
       </c>
     </row>
     <row r="83" spans="1:3" ht="12.75" x14ac:dyDescent="0.2">
@@ -3086,106 +3063,73 @@
         <v>82</v>
       </c>
       <c r="B83" s="20" t="s">
-        <v>184</v>
+        <v>173</v>
       </c>
       <c r="C83" s="33" t="s">
-        <v>185</v>
-      </c>
-    </row>
-    <row r="84" spans="1:3" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A84" s="29" t="s">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="84" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A84" s="34" t="s">
         <v>84</v>
       </c>
-      <c r="B84" s="20" t="s">
-        <v>186</v>
-      </c>
-      <c r="C84" s="33" t="s">
-        <v>187</v>
-      </c>
-    </row>
-    <row r="85" spans="1:3" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A85" s="29" t="s">
-        <v>86</v>
-      </c>
-      <c r="B85" s="20" t="s">
-        <v>188</v>
-      </c>
-      <c r="C85" s="33" t="s">
-        <v>189</v>
-      </c>
+      <c r="B84" s="35" t="s">
+        <v>175</v>
+      </c>
+      <c r="C84" s="36" t="s">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="85" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A85" s="34" t="s">
+        <v>219</v>
+      </c>
+      <c r="B85" s="41" t="s">
+        <v>94</v>
+      </c>
+      <c r="C85" s="42"/>
     </row>
     <row r="86" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A86" s="34" t="s">
-        <v>88</v>
-      </c>
-      <c r="B86" s="35" t="s">
-        <v>190</v>
-      </c>
-      <c r="C86" s="36" t="s">
-        <v>191</v>
+      <c r="A86" s="29" t="s">
+        <v>222</v>
+      </c>
+      <c r="B86" s="11"/>
+      <c r="C86" s="30" t="s">
+        <v>223</v>
       </c>
     </row>
     <row r="87" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A87" s="34" t="s">
-        <v>234</v>
-      </c>
-      <c r="B87" s="41" t="s">
-        <v>101</v>
-      </c>
-      <c r="C87" s="42"/>
+        <v>224</v>
+      </c>
+      <c r="B87" s="41"/>
+      <c r="C87" s="42" t="s">
+        <v>225</v>
+      </c>
     </row>
     <row r="88" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A88" s="29" t="s">
-        <v>238</v>
-      </c>
-      <c r="B88" s="11"/>
-      <c r="C88" s="30" t="s">
-        <v>239</v>
+      <c r="A88" s="34" t="s">
+        <v>228</v>
+      </c>
+      <c r="B88" s="41"/>
+      <c r="C88" s="42" t="s">
+        <v>229</v>
       </c>
     </row>
     <row r="89" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A89" s="34" t="s">
-        <v>240</v>
-      </c>
-      <c r="B89" s="41"/>
-      <c r="C89" s="42" t="s">
-        <v>241</v>
-      </c>
-    </row>
-    <row r="90" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A90" s="34" t="s">
-        <v>244</v>
-      </c>
-      <c r="B90" s="41"/>
-      <c r="C90" s="42" t="s">
-        <v>245</v>
-      </c>
-    </row>
-    <row r="91" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A91" s="29" t="s">
-        <v>246</v>
-      </c>
-      <c r="B91" s="15" t="s">
-        <v>114</v>
-      </c>
-      <c r="C91" s="6" t="s">
-        <v>115</v>
-      </c>
-    </row>
-    <row r="92" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A92" s="29" t="s">
-        <v>247</v>
-      </c>
-      <c r="B92" s="11" t="s">
-        <v>248</v>
-      </c>
-      <c r="C92" s="42"/>
+      <c r="A89" s="29" t="s">
+        <v>230</v>
+      </c>
+      <c r="B89" s="11" t="s">
+        <v>231</v>
+      </c>
+      <c r="C89" s="42"/>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="C75" r:id="rId1" xr:uid="{00000000-0004-0000-0100-000000000000}"/>
-    <hyperlink ref="C76" r:id="rId2" xr:uid="{00000000-0004-0000-0100-000001000000}"/>
-    <hyperlink ref="C78" r:id="rId3" xr:uid="{00000000-0004-0000-0100-000002000000}"/>
+    <hyperlink ref="C73" r:id="rId1" xr:uid="{00000000-0004-0000-0100-000000000000}"/>
+    <hyperlink ref="C74" r:id="rId2" xr:uid="{00000000-0004-0000-0100-000001000000}"/>
+    <hyperlink ref="C76" r:id="rId3" xr:uid="{00000000-0004-0000-0100-000002000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <tableParts count="1">
@@ -3216,183 +3160,183 @@
   <sheetData>
     <row r="2" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B2" s="43" t="s">
-        <v>192</v>
+        <v>177</v>
       </c>
       <c r="C2" s="44"/>
       <c r="D2" s="44"/>
       <c r="E2" s="44"/>
       <c r="G2" s="43" t="s">
-        <v>193</v>
+        <v>178</v>
       </c>
       <c r="H2" s="44"/>
       <c r="I2" s="44"/>
     </row>
     <row r="4" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B4" s="40" t="s">
-        <v>194</v>
+        <v>179</v>
       </c>
       <c r="C4" s="40" t="s">
-        <v>195</v>
+        <v>180</v>
       </c>
       <c r="D4" s="40" t="s">
-        <v>196</v>
+        <v>181</v>
       </c>
       <c r="E4" s="40" t="s">
-        <v>197</v>
+        <v>182</v>
       </c>
       <c r="G4" s="40" t="s">
-        <v>198</v>
+        <v>183</v>
       </c>
       <c r="H4" s="21"/>
       <c r="I4" s="40" t="s">
-        <v>199</v>
+        <v>184</v>
       </c>
     </row>
     <row r="5" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B5" s="17" t="s">
-        <v>200</v>
+        <v>185</v>
       </c>
       <c r="C5" s="22" t="s">
-        <v>201</v>
+        <v>186</v>
       </c>
       <c r="D5" s="18" t="s">
-        <v>202</v>
+        <v>187</v>
       </c>
       <c r="E5" s="17" t="s">
-        <v>203</v>
+        <v>188</v>
       </c>
       <c r="G5" s="9" t="s">
-        <v>204</v>
+        <v>189</v>
       </c>
       <c r="H5" s="21"/>
       <c r="I5" s="23" t="s">
-        <v>205</v>
+        <v>190</v>
       </c>
     </row>
     <row r="6" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B6" s="18" t="s">
-        <v>206</v>
+        <v>191</v>
       </c>
       <c r="C6" s="3" t="s">
-        <v>207</v>
+        <v>192</v>
       </c>
       <c r="D6" s="18" t="s">
-        <v>101</v>
+        <v>94</v>
       </c>
       <c r="E6" s="18" t="s">
-        <v>208</v>
+        <v>193</v>
       </c>
       <c r="G6" s="9" t="s">
-        <v>209</v>
+        <v>194</v>
       </c>
       <c r="H6" s="21"/>
       <c r="I6" s="23" t="s">
-        <v>210</v>
+        <v>195</v>
       </c>
     </row>
     <row r="7" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B7" s="18" t="s">
-        <v>211</v>
+        <v>196</v>
       </c>
       <c r="C7" s="22" t="s">
-        <v>212</v>
+        <v>197</v>
       </c>
       <c r="D7" s="17"/>
       <c r="E7" s="18" t="s">
-        <v>213</v>
+        <v>198</v>
       </c>
       <c r="G7" s="9" t="s">
-        <v>214</v>
+        <v>199</v>
       </c>
       <c r="H7" s="21"/>
       <c r="I7" s="23" t="s">
-        <v>215</v>
+        <v>200</v>
       </c>
     </row>
     <row r="8" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B8" s="18" t="s">
-        <v>216</v>
+        <v>201</v>
       </c>
       <c r="C8" s="3" t="s">
-        <v>217</v>
+        <v>202</v>
       </c>
       <c r="D8" s="17"/>
       <c r="E8" s="17"/>
       <c r="G8" s="9" t="s">
-        <v>218</v>
+        <v>203</v>
       </c>
       <c r="H8" s="21"/>
       <c r="I8" s="23" t="s">
-        <v>219</v>
+        <v>204</v>
       </c>
     </row>
     <row r="9" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B9" s="3" t="s">
-        <v>220</v>
+        <v>205</v>
       </c>
       <c r="C9" s="22" t="s">
-        <v>221</v>
+        <v>206</v>
       </c>
       <c r="D9" s="7"/>
       <c r="E9" s="7"/>
       <c r="G9" s="9" t="s">
-        <v>222</v>
+        <v>207</v>
       </c>
       <c r="H9" s="21"/>
       <c r="I9" s="23" t="s">
-        <v>223</v>
+        <v>208</v>
       </c>
     </row>
     <row r="10" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B10" s="7"/>
       <c r="C10" s="3" t="s">
-        <v>224</v>
+        <v>209</v>
       </c>
       <c r="D10" s="7"/>
       <c r="E10" s="7"/>
       <c r="G10" s="9" t="s">
-        <v>225</v>
+        <v>210</v>
       </c>
       <c r="H10" s="21"/>
       <c r="I10" s="23" t="s">
-        <v>226</v>
+        <v>211</v>
       </c>
     </row>
     <row r="11" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B11" s="7"/>
       <c r="C11" s="22" t="s">
-        <v>227</v>
+        <v>212</v>
       </c>
       <c r="D11" s="7"/>
       <c r="E11" s="7"/>
       <c r="G11" s="9" t="s">
-        <v>228</v>
+        <v>213</v>
       </c>
       <c r="H11" s="21"/>
       <c r="I11" s="23" t="s">
-        <v>229</v>
+        <v>214</v>
       </c>
     </row>
     <row r="12" spans="2:9" x14ac:dyDescent="0.2">
       <c r="G12" s="9" t="s">
-        <v>230</v>
+        <v>215</v>
       </c>
       <c r="I12" s="23" t="s">
-        <v>231</v>
+        <v>216</v>
       </c>
     </row>
     <row r="13" spans="2:9" x14ac:dyDescent="0.2">
       <c r="G13" s="9" t="s">
-        <v>249</v>
+        <v>232</v>
       </c>
       <c r="I13" s="23" t="s">
-        <v>232</v>
+        <v>217</v>
       </c>
     </row>
     <row r="14" spans="2:9" x14ac:dyDescent="0.2">
       <c r="G14" s="10"/>
       <c r="I14" s="23" t="s">
-        <v>233</v>
+        <v>218</v>
       </c>
     </row>
   </sheetData>

</xml_diff>